<commit_message>
Commit depois de muito tempo
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>Hoje</t>
   </si>
@@ -46,52 +46,40 @@
     <t>Opções</t>
   </si>
   <si>
-    <t>29-08-2022</t>
+    <t>15-02-2023</t>
   </si>
   <si>
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>17/08/2022  12:31:13</t>
-  </si>
-  <si>
-    <t>17/08/2022  12:39:31</t>
-  </si>
-  <si>
-    <t>17/08/2022  13:13:51</t>
-  </si>
-  <si>
-    <t>17/08/2022  15:08:14</t>
-  </si>
-  <si>
-    <t>17/08/2022  17:39:39</t>
-  </si>
-  <si>
-    <t>CLEUZA CRISTINA CARVALHO DE SOUZA</t>
-  </si>
-  <si>
-    <t>JOAO GABRIEL DE OLIVEIRA FERNANDES</t>
-  </si>
-  <si>
-    <t>HEITOR RODRIGUES DA SILVA GOMES</t>
-  </si>
-  <si>
-    <t>CAMILA ALVES BRANDÃO DE AGUIAR</t>
-  </si>
-  <si>
-    <t>CONCEIÇÃO APARECIDA COSTA DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>3 dias úteis</t>
+    <t>14/02/2023  15:30:29</t>
+  </si>
+  <si>
+    <t>15/02/2023  09:41:19</t>
+  </si>
+  <si>
+    <t>15/02/2023  12:01:13</t>
+  </si>
+  <si>
+    <t>MARIA EMILIA FONSECA RODRIGUES</t>
+  </si>
+  <si>
+    <t>DALILA DE OLIVEIRA SILVA</t>
+  </si>
+  <si>
+    <t>VIVIANE KARINE SANTOS</t>
+  </si>
+  <si>
+    <t>10 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
+    <t>Assistencial</t>
+  </si>
+  <si>
     <t>No Assistencial</t>
-  </si>
-  <si>
-    <t>Assistencial</t>
   </si>
   <si>
     <t>Responder  Detalhes</t>
@@ -452,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,25 +489,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>5798816</v>
+        <v>12092359</v>
       </c>
       <c r="E2">
-        <v>8198342</v>
+        <v>8514904</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -533,25 +521,25 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>5798847</v>
+        <v>12093061</v>
       </c>
       <c r="E3">
-        <v>8198366</v>
+        <v>8515747</v>
       </c>
       <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" t="s">
         <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -565,89 +553,25 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>5798945</v>
+        <v>12093493</v>
       </c>
       <c r="E4">
-        <v>8198504</v>
+        <v>8516300</v>
       </c>
       <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" t="s">
         <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>5799351</v>
-      </c>
-      <c r="E5">
-        <v>8198990</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>5799874</v>
-      </c>
-      <c r="E6">
-        <v>8199609</v>
-      </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustei os tempos de espera e separei a def Gender
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
   <si>
     <t>Hoje</t>
   </si>
@@ -49,37 +49,70 @@
     <t>11-04-2023</t>
   </si>
   <si>
-    <t>417823 - PREMIUM SAÚDE S.A</t>
-  </si>
-  <si>
-    <t>10/04/2023  09:19:30</t>
-  </si>
-  <si>
-    <t>10/04/2023  10:47:50</t>
-  </si>
-  <si>
-    <t>11/04/2023  08:39:19</t>
-  </si>
-  <si>
-    <t>11/04/2023  11:09:14</t>
-  </si>
-  <si>
-    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
-  </si>
-  <si>
-    <t>DIEGO SANTOS DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>AYLA ALVES COELHO</t>
-  </si>
-  <si>
-    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
+    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
+  </si>
+  <si>
+    <t>10/04/2023  08:44:11</t>
+  </si>
+  <si>
+    <t>10/04/2023  11:56:29</t>
+  </si>
+  <si>
+    <t>10/04/2023  13:25:58</t>
+  </si>
+  <si>
+    <t>10/04/2023  14:54:09</t>
+  </si>
+  <si>
+    <t>10/04/2023  15:00:01</t>
+  </si>
+  <si>
+    <t>11/04/2023  08:23:00</t>
+  </si>
+  <si>
+    <t>11/04/2023  09:34:28</t>
+  </si>
+  <si>
+    <t>11/04/2023  13:50:53</t>
+  </si>
+  <si>
+    <t>11/04/2023  15:08:53</t>
+  </si>
+  <si>
+    <t>BRAYAN MIGUEL JAFFRA PEREIRA</t>
+  </si>
+  <si>
+    <t>JANAINA MARIA DA SILVA</t>
+  </si>
+  <si>
+    <t>CLEO DALSIOR VOM DOELINGER</t>
+  </si>
+  <si>
+    <t>WELLINGTON FERREIRA DE JESUS</t>
+  </si>
+  <si>
+    <t>BENICIO MARTINS FERNANDES</t>
+  </si>
+  <si>
+    <t>PAOLA MONIQUE DA SILVA TEIXEIRA</t>
+  </si>
+  <si>
+    <t>IDEILDO LUCENA MOURA DA SILVA JUNIOR</t>
+  </si>
+  <si>
+    <t>MARIA DA CONCEICAO DA SILVA</t>
+  </si>
+  <si>
+    <t>VALDIR FERNANDES DE ARAUJO</t>
   </si>
   <si>
     <t>10 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>No Assistencial</t>
   </si>
   <si>
     <t>Assistencial</t>
@@ -443,7 +476,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,25 +525,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12161100</v>
+        <v>12161017</v>
       </c>
       <c r="E2">
-        <v>8597675</v>
+        <v>8597595</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -524,25 +557,25 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>12161386</v>
+        <v>12161650</v>
       </c>
       <c r="E3">
-        <v>8598016</v>
+        <v>8598342</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -556,25 +589,25 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>12163407</v>
+        <v>12162010</v>
       </c>
       <c r="E4">
-        <v>8600473</v>
+        <v>8598761</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -588,25 +621,185 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>12163869</v>
+        <v>12162415</v>
       </c>
       <c r="E5">
-        <v>8601052</v>
+        <v>8599264</v>
       </c>
       <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>12162439</v>
+      </c>
+      <c r="E6">
+        <v>8599230</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>12163370</v>
+      </c>
+      <c r="E7">
+        <v>8600412</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>12163535</v>
+      </c>
+      <c r="E8">
+        <v>8600621</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="D9">
+        <v>12164502</v>
+      </c>
+      <c r="E9">
+        <v>8601769</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
+      <c r="D10">
+        <v>12164852</v>
+      </c>
+      <c r="E10">
+        <v>8602234</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
migrei a def TEXTO para o rquivo Utils.py
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Hoje</t>
   </si>
@@ -49,70 +49,19 @@
     <t>11-04-2023</t>
   </si>
   <si>
-    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
-  </si>
-  <si>
-    <t>10/04/2023  08:44:11</t>
-  </si>
-  <si>
-    <t>10/04/2023  11:56:29</t>
-  </si>
-  <si>
-    <t>10/04/2023  13:25:58</t>
-  </si>
-  <si>
-    <t>10/04/2023  14:54:09</t>
-  </si>
-  <si>
-    <t>10/04/2023  15:00:01</t>
-  </si>
-  <si>
-    <t>11/04/2023  08:23:00</t>
-  </si>
-  <si>
-    <t>11/04/2023  09:34:28</t>
-  </si>
-  <si>
-    <t>11/04/2023  13:50:53</t>
-  </si>
-  <si>
-    <t>11/04/2023  15:08:53</t>
-  </si>
-  <si>
-    <t>BRAYAN MIGUEL JAFFRA PEREIRA</t>
-  </si>
-  <si>
-    <t>JANAINA MARIA DA SILVA</t>
-  </si>
-  <si>
-    <t>CLEO DALSIOR VOM DOELINGER</t>
-  </si>
-  <si>
-    <t>WELLINGTON FERREIRA DE JESUS</t>
-  </si>
-  <si>
-    <t>BENICIO MARTINS FERNANDES</t>
-  </si>
-  <si>
-    <t>PAOLA MONIQUE DA SILVA TEIXEIRA</t>
-  </si>
-  <si>
-    <t>IDEILDO LUCENA MOURA DA SILVA JUNIOR</t>
-  </si>
-  <si>
-    <t>MARIA DA CONCEICAO DA SILVA</t>
-  </si>
-  <si>
-    <t>VALDIR FERNANDES DE ARAUJO</t>
-  </si>
-  <si>
-    <t>10 dias úteis</t>
+    <t>417823 - PREMIUM SAÚDE S.A</t>
+  </si>
+  <si>
+    <t>05/04/2023  14:26:09</t>
+  </si>
+  <si>
+    <t>ANTONIO CARLOS SANTOS</t>
+  </si>
+  <si>
+    <t>8 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>No Assistencial</t>
   </si>
   <si>
     <t>Assistencial</t>
@@ -476,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -525,281 +474,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12161017</v>
+        <v>12157899</v>
       </c>
       <c r="E2">
-        <v>8597595</v>
+        <v>8593801</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>12161650</v>
-      </c>
-      <c r="E3">
-        <v>8598342</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4">
-        <v>12162010</v>
-      </c>
-      <c r="E4">
-        <v>8598761</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>12162415</v>
-      </c>
-      <c r="E5">
-        <v>8599264</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>12162439</v>
-      </c>
-      <c r="E6">
-        <v>8599230</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
         <v>17</v>
-      </c>
-      <c r="D7">
-        <v>12163370</v>
-      </c>
-      <c r="E7">
-        <v>8600412</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>12163535</v>
-      </c>
-      <c r="E8">
-        <v>8600621</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>12164502</v>
-      </c>
-      <c r="E9">
-        <v>8601769</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10">
-        <v>12164852</v>
-      </c>
-      <c r="E10">
-        <v>8602234</v>
-      </c>
-      <c r="F10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I10" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nas vers'ao anteriores tinha problema em saida.html
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Hoje</t>
   </si>
@@ -46,16 +46,22 @@
     <t>Opções</t>
   </si>
   <si>
-    <t>12-04-2023</t>
+    <t>13-04-2023</t>
   </si>
   <si>
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>06/04/2023  13:03:51</t>
-  </si>
-  <si>
-    <t>DANIELA FARIAS VASCONCELOS</t>
+    <t>10/04/2023  09:19:30</t>
+  </si>
+  <si>
+    <t>10/04/2023  10:47:50</t>
+  </si>
+  <si>
+    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
+  </si>
+  <si>
+    <t>DIEGO SANTOS DE ALMEIDA</t>
   </si>
   <si>
     <t>8 dias úteis</t>
@@ -425,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,25 +480,57 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12159646</v>
+        <v>12161100</v>
       </c>
       <c r="E2">
-        <v>7797800</v>
+        <v>8597675</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="D3">
+        <v>12161386</v>
+      </c>
+      <c r="E3">
+        <v>8598016</v>
+      </c>
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H3" t="s">
         <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrocedi ações e aprimorei o index para notebook
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="40">
   <si>
     <t>Hoje</t>
   </si>
@@ -49,22 +49,82 @@
     <t>13-04-2023</t>
   </si>
   <si>
-    <t>417823 - PREMIUM SAÚDE S.A</t>
-  </si>
-  <si>
-    <t>10/04/2023  09:19:30</t>
-  </si>
-  <si>
-    <t>10/04/2023  10:47:50</t>
-  </si>
-  <si>
-    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
-  </si>
-  <si>
-    <t>DIEGO SANTOS DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>8 dias úteis</t>
+    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
+  </si>
+  <si>
+    <t>12/04/2023  11:59:41</t>
+  </si>
+  <si>
+    <t>12/04/2023  12:03:08</t>
+  </si>
+  <si>
+    <t>12/04/2023  15:43:18</t>
+  </si>
+  <si>
+    <t>12/04/2023  16:14:52</t>
+  </si>
+  <si>
+    <t>13/04/2023  08:23:06</t>
+  </si>
+  <si>
+    <t>13/04/2023  11:42:27</t>
+  </si>
+  <si>
+    <t>13/04/2023  13:26:27</t>
+  </si>
+  <si>
+    <t>13/04/2023  15:12:39</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:38:38</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:46:57</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:58:57</t>
+  </si>
+  <si>
+    <t>13/04/2023  18:17:42</t>
+  </si>
+  <si>
+    <t>MARLENE NUNES HONDA TAVARES</t>
+  </si>
+  <si>
+    <t>MARCO ANTONIO DALPRA</t>
+  </si>
+  <si>
+    <t>RAVI SCHULZ XAVIER DA CRUZ</t>
+  </si>
+  <si>
+    <t>KAYKY BRUNNO SOUZA LOPES</t>
+  </si>
+  <si>
+    <t>MÔNICA ALVES GOMES</t>
+  </si>
+  <si>
+    <t>MARCIO CANDIDO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>BARBARA KELLY CARNEIRO LEÃO RODRIGUES</t>
+  </si>
+  <si>
+    <t>ANALIS SOARES SILVA</t>
+  </si>
+  <si>
+    <t>MAICKSON CAIQUE VENANCIO</t>
+  </si>
+  <si>
+    <t>EMILLE FERNANDES CORREA</t>
+  </si>
+  <si>
+    <t>MILENA FREIRE TRAVASSOS COUSSEIRO</t>
+  </si>
+  <si>
+    <t>ROGERIA DORALICE SOARES DA SILVA</t>
+  </si>
+  <si>
+    <t>10 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
@@ -431,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -480,25 +540,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12161100</v>
+        <v>12166383</v>
       </c>
       <c r="E2">
-        <v>8597675</v>
+        <v>8604036</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -512,25 +572,345 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>12161386</v>
+        <v>12166396</v>
       </c>
       <c r="E3">
-        <v>8598016</v>
+        <v>8604069</v>
       </c>
       <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>12167333</v>
+      </c>
+      <c r="E4">
+        <v>8605179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D5">
+        <v>12167445</v>
+      </c>
+      <c r="E5">
+        <v>8605345</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="D6">
+        <v>12168095</v>
+      </c>
+      <c r="E6">
+        <v>8606114</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="D7">
+        <v>12168687</v>
+      </c>
+      <c r="E7">
+        <v>8606848</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="D8">
+        <v>12169086</v>
+      </c>
+      <c r="E8">
+        <v>8607367</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
+      </c>
+      <c r="D9">
+        <v>12169516</v>
+      </c>
+      <c r="E9">
+        <v>8607900</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
+      </c>
+      <c r="J9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>12169806</v>
+      </c>
+      <c r="E10">
+        <v>8608265</v>
+      </c>
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>12169830</v>
+      </c>
+      <c r="E11">
+        <v>8608288</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>12169862</v>
+      </c>
+      <c r="E12">
+        <v>8608371</v>
+      </c>
+      <c r="F12" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>12170051</v>
+      </c>
+      <c r="E13">
+        <v>8608573</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustei a iamgem e título da 1a pagina
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Hoje</t>
   </si>
@@ -52,13 +52,31 @@
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>06/04/2023  13:03:51</t>
-  </si>
-  <si>
-    <t>DANIELA FARIAS VASCONCELOS</t>
-  </si>
-  <si>
-    <t>7 dias úteis</t>
+    <t>03/04/2023  13:44:27</t>
+  </si>
+  <si>
+    <t>03/04/2023  14:47:05</t>
+  </si>
+  <si>
+    <t>03/04/2023  15:25:17</t>
+  </si>
+  <si>
+    <t>03/04/2023  19:51:17</t>
+  </si>
+  <si>
+    <t>BÁRBARA DE OLIVEIRA PATRÍCIO</t>
+  </si>
+  <si>
+    <t>KEPA FREDRICK STOCKNER</t>
+  </si>
+  <si>
+    <t>DAVIDSON LUIZ PEREIRA LOPES</t>
+  </si>
+  <si>
+    <t>KENIA CLAUDIA FARIA CAMPOS</t>
+  </si>
+  <si>
+    <t>4 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
@@ -425,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,25 +492,121 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12159646</v>
+        <v>12153205</v>
       </c>
       <c r="E2">
-        <v>7797800</v>
+        <v>8588077</v>
       </c>
       <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D3">
+        <v>12153463</v>
+      </c>
+      <c r="E3">
+        <v>8588431</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="D4">
+        <v>12153630</v>
+      </c>
+      <c r="E4">
+        <v>8588645</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
+      <c r="D5">
+        <v>12154294</v>
+      </c>
+      <c r="E5">
+        <v>8589407</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dando esse commit, porém há erro ao abrir o word
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
   <si>
     <t>Hoje</t>
   </si>
@@ -46,37 +46,61 @@
     <t>Opções</t>
   </si>
   <si>
-    <t>13-04-2023</t>
-  </si>
-  <si>
-    <t>417823 - PREMIUM SAÚDE S.A</t>
-  </si>
-  <si>
-    <t>03/04/2023  13:44:27</t>
-  </si>
-  <si>
-    <t>03/04/2023  14:47:05</t>
-  </si>
-  <si>
-    <t>03/04/2023  15:25:17</t>
-  </si>
-  <si>
-    <t>03/04/2023  19:51:17</t>
-  </si>
-  <si>
-    <t>BÁRBARA DE OLIVEIRA PATRÍCIO</t>
-  </si>
-  <si>
-    <t>KEPA FREDRICK STOCKNER</t>
-  </si>
-  <si>
-    <t>DAVIDSON LUIZ PEREIRA LOPES</t>
-  </si>
-  <si>
-    <t>KENIA CLAUDIA FARIA CAMPOS</t>
-  </si>
-  <si>
-    <t>4 dias úteis</t>
+    <t>14-04-2023</t>
+  </si>
+  <si>
+    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
+  </si>
+  <si>
+    <t>13/04/2023  08:23:06</t>
+  </si>
+  <si>
+    <t>13/04/2023  11:42:27</t>
+  </si>
+  <si>
+    <t>13/04/2023  13:26:27</t>
+  </si>
+  <si>
+    <t>13/04/2023  15:12:39</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:38:38</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:46:57</t>
+  </si>
+  <si>
+    <t>13/04/2023  16:58:57</t>
+  </si>
+  <si>
+    <t>13/04/2023  18:17:42</t>
+  </si>
+  <si>
+    <t>MÔNICA ALVES GOMES</t>
+  </si>
+  <si>
+    <t>MARCIO CANDIDO DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>BARBARA KELLY CARNEIRO LEÃO RODRIGUES</t>
+  </si>
+  <si>
+    <t>ANALIS SOARES SILVA</t>
+  </si>
+  <si>
+    <t>MAICKSON CAIQUE VENANCIO</t>
+  </si>
+  <si>
+    <t>EMILLE FERNANDES CORREA</t>
+  </si>
+  <si>
+    <t>MILENA FREIRE TRAVASSOS COUSSEIRO</t>
+  </si>
+  <si>
+    <t>ROGERIA DORALICE SOARES DA SILVA</t>
+  </si>
+  <si>
+    <t>10 dias úteis</t>
   </si>
   <si>
     <t>NO</t>
@@ -443,7 +467,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,25 +516,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12153205</v>
+        <v>12168095</v>
       </c>
       <c r="E2">
-        <v>8588077</v>
+        <v>8606114</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -524,25 +548,25 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>12153463</v>
+        <v>12168687</v>
       </c>
       <c r="E3">
-        <v>8588431</v>
+        <v>8606848</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -556,25 +580,25 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>12153630</v>
+        <v>12169086</v>
       </c>
       <c r="E4">
-        <v>8588645</v>
+        <v>8607367</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -588,25 +612,153 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>12154294</v>
+        <v>12169516</v>
       </c>
       <c r="E5">
-        <v>8589407</v>
+        <v>8607900</v>
       </c>
       <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>12169806</v>
+      </c>
+      <c r="E6">
+        <v>8608265</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>12169830</v>
+      </c>
+      <c r="E7">
+        <v>8608288</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>12169862</v>
+      </c>
+      <c r="E8">
+        <v>8608371</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>23</v>
+      <c r="D9">
+        <v>12170051</v>
+      </c>
+      <c r="E9">
+        <v>8608573</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vários ajustes fiz vários teste e rodou
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Hoje</t>
   </si>
@@ -49,55 +49,43 @@
     <t>14-04-2023</t>
   </si>
   <si>
-    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
-  </si>
-  <si>
-    <t>13/04/2023  08:23:06</t>
-  </si>
-  <si>
-    <t>13/04/2023  11:42:27</t>
-  </si>
-  <si>
-    <t>13/04/2023  13:26:27</t>
-  </si>
-  <si>
-    <t>13/04/2023  15:12:39</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:38:38</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:46:57</t>
-  </si>
-  <si>
-    <t>13/04/2023  16:58:57</t>
-  </si>
-  <si>
-    <t>13/04/2023  18:17:42</t>
-  </si>
-  <si>
-    <t>MÔNICA ALVES GOMES</t>
-  </si>
-  <si>
-    <t>MARCIO CANDIDO DE OLIVEIRA</t>
-  </si>
-  <si>
-    <t>BARBARA KELLY CARNEIRO LEÃO RODRIGUES</t>
-  </si>
-  <si>
-    <t>ANALIS SOARES SILVA</t>
-  </si>
-  <si>
-    <t>MAICKSON CAIQUE VENANCIO</t>
-  </si>
-  <si>
-    <t>EMILLE FERNANDES CORREA</t>
-  </si>
-  <si>
-    <t>MILENA FREIRE TRAVASSOS COUSSEIRO</t>
-  </si>
-  <si>
-    <t>ROGERIA DORALICE SOARES DA SILVA</t>
+    <t>417823 - PREMIUM SAÚDE S.A</t>
+  </si>
+  <si>
+    <t>13/04/2023  10:06:53</t>
+  </si>
+  <si>
+    <t>13/04/2023  15:44:44</t>
+  </si>
+  <si>
+    <t>13/04/2023  17:09:35</t>
+  </si>
+  <si>
+    <t>14/04/2023  10:46:04</t>
+  </si>
+  <si>
+    <t>14/04/2023  11:24:10</t>
+  </si>
+  <si>
+    <t>14/04/2023  15:09:48</t>
+  </si>
+  <si>
+    <t>MELINDA GOULART CRUZ</t>
+  </si>
+  <si>
+    <t>JORGE EUSTACIO MEDEIROS</t>
+  </si>
+  <si>
+    <t>NATALIA SOLANO ROSSELIS PEREIRA DA SILVA</t>
+  </si>
+  <si>
+    <t>RAFAELLE FONSECA DE OLIVEIRA</t>
+  </si>
+  <si>
+    <t>VANESSA WINTER NUNES FORTES</t>
+  </si>
+  <si>
+    <t>OLIVER MIRANDA PORTO</t>
   </si>
   <si>
     <t>10 dias úteis</t>
@@ -107,6 +95,9 @@
   </si>
   <si>
     <t>Assistencial</t>
+  </si>
+  <si>
+    <t>No Assistencial</t>
   </si>
   <si>
     <t>Responder  Detalhes</t>
@@ -467,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -516,25 +507,25 @@
         <v>12</v>
       </c>
       <c r="D2">
-        <v>12168095</v>
+        <v>12168346</v>
       </c>
       <c r="E2">
-        <v>8606114</v>
+        <v>8606403</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
         <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -548,25 +539,25 @@
         <v>13</v>
       </c>
       <c r="D3">
-        <v>12168687</v>
+        <v>12169638</v>
       </c>
       <c r="E3">
-        <v>8606848</v>
+        <v>8608000</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -580,25 +571,25 @@
         <v>14</v>
       </c>
       <c r="D4">
-        <v>12169086</v>
+        <v>12169885</v>
       </c>
       <c r="E4">
-        <v>8607367</v>
+        <v>8608362</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" t="s">
         <v>28</v>
-      </c>
-      <c r="H4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -612,25 +603,25 @@
         <v>15</v>
       </c>
       <c r="D5">
-        <v>12169516</v>
+        <v>12170717</v>
       </c>
       <c r="E5">
-        <v>8607900</v>
+        <v>8609371</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J5" t="s">
         <v>28</v>
-      </c>
-      <c r="H5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -644,25 +635,25 @@
         <v>16</v>
       </c>
       <c r="D6">
-        <v>12169806</v>
+        <v>12170838</v>
       </c>
       <c r="E6">
-        <v>8608265</v>
+        <v>8609527</v>
       </c>
       <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" t="s">
         <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -676,89 +667,25 @@
         <v>17</v>
       </c>
       <c r="D7">
-        <v>12169830</v>
+        <v>12171665</v>
       </c>
       <c r="E7">
-        <v>8608288</v>
+        <v>8610551</v>
       </c>
       <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" t="s">
         <v>25</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" t="s">
         <v>28</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8">
-        <v>12169862</v>
-      </c>
-      <c r="E8">
-        <v>8608371</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
-        <v>12170051</v>
-      </c>
-      <c r="E9">
-        <v>8608573</v>
-      </c>
-      <c r="F9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Utilizai plailha ESpaço NIP para coletar demandas
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,15 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+  <si>
+    <t>Operadora</t>
+  </si>
   <si>
     <t>Hoje</t>
   </si>
   <si>
-    <t>Operadora</t>
-  </si>
-  <si>
-    <t>Data da Notificação</t>
+    <t>Notificação</t>
   </si>
   <si>
     <t>Demanda</t>
@@ -34,6 +34,12 @@
     <t>Beneficiário</t>
   </si>
   <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
     <t>Prazo</t>
   </si>
   <si>
@@ -43,43 +49,49 @@
     <t>Natureza</t>
   </si>
   <si>
-    <t>Opções</t>
-  </si>
-  <si>
-    <t>14-04-2023</t>
-  </si>
-  <si>
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>10/04/2023  09:19:30</t>
-  </si>
-  <si>
-    <t>10/04/2023  10:47:50</t>
-  </si>
-  <si>
-    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
-  </si>
-  <si>
-    <t>DIEGO SANTOS DE ALMEIDA</t>
-  </si>
-  <si>
-    <t>7 dias úteis</t>
+    <t>17-04-2023</t>
+  </si>
+  <si>
+    <t>8600473</t>
+  </si>
+  <si>
+    <t>8601052</t>
+  </si>
+  <si>
+    <t>AYLA ALVES COELHO</t>
+  </si>
+  <si>
+    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
+  </si>
+  <si>
+    <t>19014458606</t>
+  </si>
+  <si>
+    <t>10136083641</t>
+  </si>
+  <si>
+    <t>minha filha usa NEOCATE desde os 4 meses de idade, foi solicitado o pedido de intolerancia a lactose no dia 22/3/2023 porem nao tenho retorno quando ligo dizem, que pode levar ate 21 dias uteis mas em consulta ao site da ANS esse prazo seria pra procedimentos PAC, que nao e o caso de um exame de sangue para detectar intolerância a lactose, preciso de um retorno visto que o prazo de 10 dias uteis finalizou em 06/04/2023.</t>
+  </si>
+  <si>
+    <t>Solicitei com 10 dias de antecedência a marcação do exame de ultrassonografia endovaginal,na clínica Santa Helena ltda através do plano,ao chegar no estabelecimento no dia do exame a operadora do plano negou meu procedimento alegando que a clinica não estava mais cadastrada,porém não recebi nenhum contanto prévio mesmo estando com o agendamento feito a dias.</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
     <t>Assistencial</t>
-  </si>
-  <si>
-    <t>Responder  Detalhes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -132,11 +144,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,13 +444,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,69 +481,78 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45027.36063657407</v>
+      </c>
+      <c r="D2">
+        <v>12163407</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="D2">
-        <v>12161100</v>
-      </c>
-      <c r="E2">
-        <v>8597675</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="C3" s="2">
+        <v>45027.46474537037</v>
+      </c>
+      <c r="D3">
+        <v>12163869</v>
+      </c>
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3">
-        <v>12161386</v>
-      </c>
-      <c r="E3">
-        <v>8598016</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
       <c r="H3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tem campo de entrada tá func
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Operadora</t>
   </si>
@@ -49,34 +49,44 @@
     <t>Natureza</t>
   </si>
   <si>
-    <t>417823 - PREMIUM SAÚDE S.A</t>
-  </si>
-  <si>
-    <t>17-04-2023</t>
-  </si>
-  <si>
-    <t>8600473</t>
-  </si>
-  <si>
-    <t>8601052</t>
-  </si>
-  <si>
-    <t>AYLA ALVES COELHO</t>
-  </si>
-  <si>
-    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
-  </si>
-  <si>
-    <t>19014458606</t>
-  </si>
-  <si>
-    <t>10136083641</t>
-  </si>
-  <si>
-    <t>minha filha usa NEOCATE desde os 4 meses de idade, foi solicitado o pedido de intolerancia a lactose no dia 22/3/2023 porem nao tenho retorno quando ligo dizem, que pode levar ate 21 dias uteis mas em consulta ao site da ANS esse prazo seria pra procedimentos PAC, que nao e o caso de um exame de sangue para detectar intolerância a lactose, preciso de um retorno visto que o prazo de 10 dias uteis finalizou em 06/04/2023.</t>
-  </si>
-  <si>
-    <t>Solicitei com 10 dias de antecedência a marcação do exame de ultrassonografia endovaginal,na clínica Santa Helena ltda através do plano,ao chegar no estabelecimento no dia do exame a operadora do plano negou meu procedimento alegando que a clinica não estava mais cadastrada,porém não recebi nenhum contanto prévio mesmo estando com o agendamento feito a dias.</t>
+    <t>Contrato</t>
+  </si>
+  <si>
+    <t>Registro</t>
+  </si>
+  <si>
+    <t>Modalidade</t>
+  </si>
+  <si>
+    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
+  </si>
+  <si>
+    <t>18-04-2023</t>
+  </si>
+  <si>
+    <t>8595238</t>
+  </si>
+  <si>
+    <t>8596884</t>
+  </si>
+  <si>
+    <t>CARLOS RODRIGO CHAGAS GITIRANA</t>
+  </si>
+  <si>
+    <t>CRISTIANO DE OLIVEIRA CARNEIRO</t>
+  </si>
+  <si>
+    <t>04466559457</t>
+  </si>
+  <si>
+    <t>87895145487</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dia 22/03/2023 eu solicitei autorização para o exame de colonoscopia com biópsia, já se passaram 10 dias úteis e ainda não foi autorizado </t>
+  </si>
+  <si>
+    <t>Fiz a migração do plano Hapvida para o you saúde,  e foi nos garantido a redução das carências pela corretora de saúde e quando precisei de exames não foi autorizada. Entrei em contato com a you saúde e a administradora Sindfort e não deram solução._x000D_
+Obs entreguei todos os documentos solicitados no início de janeiro e nada. Estou sendo enganado e lesado .</t>
   </si>
   <si>
     <t>NO</t>
@@ -444,13 +454,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -484,75 +494,84 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>45027.36063657407</v>
+        <v>45022.40521990741</v>
       </c>
       <c r="D2">
-        <v>12163407</v>
+        <v>12159014</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3" s="2">
+        <v>45022.71378472223</v>
+      </c>
+      <c r="D3">
+        <v>12160376</v>
+      </c>
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45027.46474537037</v>
-      </c>
-      <c r="D3">
-        <v>12163869</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I3">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="K3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Novo commit depois bug Word
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -58,35 +58,34 @@
     <t>Modalidade</t>
   </si>
   <si>
-    <t>422380 - YOU ASSISTÊNCIA MÉDICA LTDA</t>
+    <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
     <t>18-04-2023</t>
   </si>
   <si>
-    <t>8595238</t>
-  </si>
-  <si>
-    <t>8596884</t>
-  </si>
-  <si>
-    <t>CARLOS RODRIGO CHAGAS GITIRANA</t>
-  </si>
-  <si>
-    <t>CRISTIANO DE OLIVEIRA CARNEIRO</t>
-  </si>
-  <si>
-    <t>04466559457</t>
-  </si>
-  <si>
-    <t>87895145487</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No dia 22/03/2023 eu solicitei autorização para o exame de colonoscopia com biópsia, já se passaram 10 dias úteis e ainda não foi autorizado </t>
-  </si>
-  <si>
-    <t>Fiz a migração do plano Hapvida para o you saúde,  e foi nos garantido a redução das carências pela corretora de saúde e quando precisei de exames não foi autorizada. Entrei em contato com a you saúde e a administradora Sindfort e não deram solução._x000D_
-Obs entreguei todos os documentos solicitados no início de janeiro e nada. Estou sendo enganado e lesado .</t>
+    <t>8600473</t>
+  </si>
+  <si>
+    <t>8601052</t>
+  </si>
+  <si>
+    <t>AYLA ALVES COELHO</t>
+  </si>
+  <si>
+    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
+  </si>
+  <si>
+    <t>19014458606</t>
+  </si>
+  <si>
+    <t>10136083641</t>
+  </si>
+  <si>
+    <t>minha filha usa NEOCATE desde os 4 meses de idade, foi solicitado o pedido de intolerancia a lactose no dia 22/3/2023 porem nao tenho retorno quando ligo dizem, que pode levar ate 21 dias uteis mas em consulta ao site da ANS esse prazo seria pra procedimentos PAC, que nao e o caso de um exame de sangue para detectar intolerância a lactose, preciso de um retorno visto que o prazo de 10 dias uteis finalizou em 06/04/2023.</t>
+  </si>
+  <si>
+    <t>Solicitei com 10 dias de antecedência a marcação do exame de ultrassonografia endovaginal,na clínica Santa Helena ltda através do plano,ao chegar no estabelecimento no dia do exame a operadora do plano negou meu procedimento alegando que a clinica não estava mais cadastrada,porém não recebi nenhum contanto prévio mesmo estando com o agendamento feito a dias.</t>
   </si>
   <si>
     <t>NO</t>
@@ -512,10 +511,10 @@
         <v>15</v>
       </c>
       <c r="C2" s="2">
-        <v>45022.40521990741</v>
+        <v>45027.36063657407</v>
       </c>
       <c r="D2">
-        <v>12159014</v>
+        <v>12163407</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
@@ -530,7 +529,7 @@
         <v>22</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>24</v>
@@ -547,10 +546,10 @@
         <v>15</v>
       </c>
       <c r="C3" s="2">
-        <v>45022.71378472223</v>
+        <v>45027.46474537037</v>
       </c>
       <c r="D3">
-        <v>12160376</v>
+        <v>12163869</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -565,7 +564,7 @@
         <v>23</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Consegui gravar Contrato, Modalidade e Registro
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Operadora</t>
   </si>
@@ -58,30 +58,27 @@
     <t>Modalidade</t>
   </si>
   <si>
+    <t>contrato</t>
+  </si>
+  <si>
+    <t>modalidade</t>
+  </si>
+  <si>
+    <t>registro</t>
+  </si>
+  <si>
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
     <t>18-04-2023</t>
   </si>
   <si>
-    <t>8600473</t>
-  </si>
-  <si>
-    <t>8601052</t>
-  </si>
-  <si>
     <t>AYLA ALVES COELHO</t>
   </si>
   <si>
     <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
   </si>
   <si>
-    <t>19014458606</t>
-  </si>
-  <si>
-    <t>10136083641</t>
-  </si>
-  <si>
     <t>minha filha usa NEOCATE desde os 4 meses de idade, foi solicitado o pedido de intolerancia a lactose no dia 22/3/2023 porem nao tenho retorno quando ligo dizem, que pode levar ate 21 dias uteis mas em consulta ao site da ANS esse prazo seria pra procedimentos PAC, que nao e o caso de um exame de sangue para detectar intolerância a lactose, preciso de um retorno visto que o prazo de 10 dias uteis finalizou em 06/04/2023.</t>
   </si>
   <si>
@@ -92,6 +89,18 @@
   </si>
   <si>
     <t>Assistencial</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>naghsfghsfgn</t>
+  </si>
+  <si>
+    <t>nsfghsan</t>
+  </si>
+  <si>
+    <t>nasghshn</t>
   </si>
 </sst>
 </file>
@@ -453,13 +462,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,13 +511,22 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2">
         <v>45027.36063657407</v>
@@ -516,34 +534,43 @@
       <c r="D2">
         <v>12163407</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
+      <c r="E2">
+        <v>8600473</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>19014458606</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I2">
         <v>6</v>
       </c>
       <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
       </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2">
         <v>45027.46474537037</v>
@@ -551,26 +578,35 @@
       <c r="D3">
         <v>12163869</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
+      <c r="E3">
+        <v>8601052</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>10136083641</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3">
         <v>6</v>
       </c>
       <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" t="s">
-        <v>25</v>
+      <c r="O3" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mais ajustes em Cont. Modali. Registro
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Operadora</t>
   </si>
@@ -58,31 +58,22 @@
     <t>Modalidade</t>
   </si>
   <si>
-    <t>contrato</t>
-  </si>
-  <si>
-    <t>modalidade</t>
-  </si>
-  <si>
-    <t>registro</t>
-  </si>
-  <si>
     <t>417823 - PREMIUM SAÚDE S.A</t>
   </si>
   <si>
-    <t>18-04-2023</t>
-  </si>
-  <si>
-    <t>AYLA ALVES COELHO</t>
-  </si>
-  <si>
-    <t>PRISCILA APARECIDA SANTOS FRANCISCO</t>
-  </si>
-  <si>
-    <t>minha filha usa NEOCATE desde os 4 meses de idade, foi solicitado o pedido de intolerancia a lactose no dia 22/3/2023 porem nao tenho retorno quando ligo dizem, que pode levar ate 21 dias uteis mas em consulta ao site da ANS esse prazo seria pra procedimentos PAC, que nao e o caso de um exame de sangue para detectar intolerância a lactose, preciso de um retorno visto que o prazo de 10 dias uteis finalizou em 06/04/2023.</t>
-  </si>
-  <si>
-    <t>Solicitei com 10 dias de antecedência a marcação do exame de ultrassonografia endovaginal,na clínica Santa Helena ltda através do plano,ao chegar no estabelecimento no dia do exame a operadora do plano negou meu procedimento alegando que a clinica não estava mais cadastrada,porém não recebi nenhum contanto prévio mesmo estando com o agendamento feito a dias.</t>
+    <t>19-04-2023</t>
+  </si>
+  <si>
+    <t>CAIO HENRIQUE RODRIGUES FERNANDES</t>
+  </si>
+  <si>
+    <t>DIEGO SANTOS DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>Interlocutora que se identifica como mãe do beneficiário, questiona a falta de atendimento para Consulta com Otorrinolaringologista, Audiometria Tonal e Vocal, Impedanciometria, Videoendoscopia nasossinusal. A solicitação foi feita à Operadora no dia 23/03/2023, para realização no município BETIM. A operadora não apresenta resposta ao pedido, informou apenas que buscaria profissional. Protocolo: 3682532023041042947 - Data: 10/04/2023.</t>
+  </si>
+  <si>
+    <t>Interlocutora, que se identifica como esposa  do beneficiário, questiona a falta de atendimento para cartão com orçamento e valores dos matérias para cirurgia  reconstrução do ligamento cruzado anterior  . A solicitação foi feita à Operadora em julho/2022, para realização no município patos de minas . A operadora  não apresenta resposta ao pedido, operadora já lhe encaminhou uma carta mas não esta\ com os valores dos matérias com o hospital deseja    Protocolo:36825320230410426644 data:1/04/2023.</t>
   </si>
   <si>
     <t>NO</t>
@@ -91,16 +82,22 @@
     <t>Assistencial</t>
   </si>
   <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>naghsfghsfgn</t>
-  </si>
-  <si>
-    <t>nsfghsan</t>
-  </si>
-  <si>
-    <t>nasghshn</t>
+    <t>Cláudio</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Vieira</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Amantino</t>
+  </si>
+  <si>
+    <t>Batista</t>
   </si>
 </sst>
 </file>
@@ -462,13 +459,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,102 +508,93 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="B2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="C2" s="2">
+        <v>45026.38854166667</v>
+      </c>
+      <c r="D2">
+        <v>12161100</v>
+      </c>
+      <c r="E2">
+        <v>8597675</v>
+      </c>
+      <c r="F2" t="s">
         <v>16</v>
       </c>
+      <c r="G2">
+        <v>17042707664</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45026.44988425926</v>
+      </c>
+      <c r="D3">
+        <v>12161386</v>
+      </c>
+      <c r="E3">
+        <v>8598016</v>
+      </c>
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2">
-        <v>45027.36063657407</v>
-      </c>
-      <c r="D2">
-        <v>12163407</v>
-      </c>
-      <c r="E2">
-        <v>8600473</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G3">
+        <v>1990602665</v>
+      </c>
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
-        <v>19014458606</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="M3" t="s">
         <v>25</v>
       </c>
-      <c r="P2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45027.46474537037</v>
-      </c>
-      <c r="D3">
-        <v>12163869</v>
-      </c>
-      <c r="E3">
-        <v>8601052</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>10136083641</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" t="s">
+      <c r="N3" t="s">
         <v>27</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ainda ajustando campos de entrda
</commit_message>
<xml_diff>
--- a/planilha/responder.xlsx
+++ b/planilha/responder.xlsx
@@ -88,16 +88,16 @@
     <t>44</t>
   </si>
   <si>
-    <t>22</t>
+    <t>33</t>
+  </si>
+  <si>
+    <t>666ert</t>
+  </si>
+  <si>
+    <t>222</t>
   </si>
   <si>
     <t>55</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>66</t>
   </si>
 </sst>
 </file>

</xml_diff>